<commit_message>
manuscript sent to Brian
</commit_message>
<xml_diff>
--- a/data/vrmid1/raw/VRMID subject notes.xlsx
+++ b/data/vrmid1/raw/VRMID subject notes.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rh/Desktop/VRMID-analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanyan/Desktop/VRMID-analysis/mid-pupil/data/vrmid1/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F90C34-9799-AD4D-B40D-1C07C90EA72E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A0589B-43E0-8749-949B-10536F8365B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17000" yWindow="1760" windowWidth="35840" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="110">
   <si>
     <t>name</t>
   </si>
@@ -345,6 +358,12 @@
   </si>
   <si>
     <t>went black</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>gender</t>
   </si>
 </sst>
 </file>
@@ -625,37 +644,42 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -667,14 +691,15 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -686,14 +711,15 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -706,20 +732,23 @@
       <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4">
+        <v>22</v>
+      </c>
+      <c r="F4" s="3">
         <v>44820</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="4">
         <v>0.52083333333333337</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>24</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -732,20 +761,23 @@
       <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5">
+        <v>29</v>
+      </c>
+      <c r="F5" s="3">
         <v>44820</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="4">
         <v>0.60416666666666663</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>62</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -758,20 +790,23 @@
       <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6">
+        <v>24</v>
+      </c>
+      <c r="F6" s="3">
         <v>44823</v>
       </c>
-      <c r="F6" s="4">
+      <c r="G6" s="4">
         <v>0.4375</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>23</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>18</v>
@@ -782,20 +817,23 @@
       <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7">
+        <v>19</v>
+      </c>
+      <c r="F7" s="3">
         <v>44860</v>
       </c>
-      <c r="F7" s="4">
+      <c r="G7" s="4">
         <v>0.45833333333333331</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>25</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>21</v>
@@ -806,20 +844,23 @@
       <c r="D8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8">
+        <v>25</v>
+      </c>
+      <c r="F8" s="3">
         <v>44865</v>
       </c>
-      <c r="F8" s="4">
+      <c r="G8" s="4">
         <v>0.50902777777777775</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>34</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>23</v>
@@ -830,23 +871,26 @@
       <c r="D9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9">
+        <v>24</v>
+      </c>
+      <c r="F9" s="3">
         <v>44872</v>
       </c>
-      <c r="F9" s="4">
+      <c r="G9" s="4">
         <v>0.56805555555555554</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <v>30</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="I9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>25</v>
@@ -857,20 +901,23 @@
       <c r="D10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="F10" s="3">
         <v>44873</v>
       </c>
-      <c r="F10" s="4">
+      <c r="G10" s="4">
         <v>0.59791666666666665</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <v>30</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>27</v>
@@ -881,23 +928,26 @@
       <c r="D11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11">
+        <v>21</v>
+      </c>
+      <c r="F11" s="3">
         <v>44873</v>
       </c>
-      <c r="F11" s="4">
+      <c r="G11" s="4">
         <v>0.63958333333333328</v>
       </c>
-      <c r="G11" s="1">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="1">
         <v>20</v>
       </c>
       <c r="I11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>30</v>
@@ -908,20 +958,23 @@
       <c r="D12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12">
+        <v>30</v>
+      </c>
+      <c r="F12" s="3">
         <v>44876</v>
       </c>
-      <c r="F12" s="4">
+      <c r="G12" s="4">
         <v>0.49375000000000002</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <v>29</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>32</v>
@@ -932,20 +985,23 @@
       <c r="D13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13">
+        <v>21</v>
+      </c>
+      <c r="F13" s="3">
         <v>44896</v>
       </c>
-      <c r="F13" s="4">
+      <c r="G13" s="4">
         <v>0.5625</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <v>25</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>35</v>
@@ -956,31 +1012,34 @@
       <c r="D14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14">
+        <v>20</v>
+      </c>
+      <c r="F14" s="3">
         <v>44896</v>
       </c>
-      <c r="F14" s="4">
+      <c r="G14" s="4">
         <v>0.61111111111111116</v>
       </c>
-      <c r="G14" s="1">
-        <v>40</v>
-      </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="1">
+        <v>40</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F15" s="3"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
         <v>4</v>
       </c>
@@ -993,17 +1052,20 @@
       <c r="D16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16">
+        <v>20</v>
+      </c>
+      <c r="F16" s="3">
         <v>44897</v>
       </c>
-      <c r="F16" s="4">
+      <c r="G16" s="4">
         <v>0.99375000000000002</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H16" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
         <v>5</v>
       </c>
@@ -1016,20 +1078,23 @@
       <c r="D17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17">
+        <v>22</v>
+      </c>
+      <c r="F17" s="3">
         <v>44897</v>
       </c>
-      <c r="F17" s="4">
+      <c r="G17" s="4">
         <v>0.52083333333333337</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
         <v>38</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
         <v>6</v>
       </c>
@@ -1042,17 +1107,20 @@
       <c r="D18" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18">
+        <v>21</v>
+      </c>
+      <c r="F18" s="3">
         <v>44897</v>
       </c>
-      <c r="F18" s="4">
+      <c r="G18" s="4">
         <v>0.5625</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
         <v>7</v>
       </c>
@@ -1065,23 +1133,23 @@
       <c r="D19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="3">
+      <c r="F19" s="3">
         <v>44901</v>
       </c>
-      <c r="F19" s="4">
+      <c r="G19" s="4">
         <v>0.40625</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <v>34</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="I19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
         <v>51</v>
@@ -1092,20 +1160,23 @@
       <c r="D20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20">
+        <v>33</v>
+      </c>
+      <c r="F20" s="3">
         <v>44902</v>
       </c>
-      <c r="F20" s="4">
+      <c r="G20" s="4">
         <v>0.375</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H20" s="1">
         <v>35</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
         <v>8</v>
       </c>
@@ -1118,20 +1189,23 @@
       <c r="D21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21">
+        <v>19</v>
+      </c>
+      <c r="F21" s="3">
         <v>44902</v>
       </c>
-      <c r="F21" s="4">
+      <c r="G21" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H21" s="1">
         <v>31</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I21" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
         <v>9</v>
       </c>
@@ -1144,20 +1218,23 @@
       <c r="D22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22">
+        <v>20</v>
+      </c>
+      <c r="F22" s="3">
         <v>44902</v>
       </c>
-      <c r="F22" s="4">
+      <c r="G22" s="4">
         <v>0.5</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H22" s="1">
         <v>30</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I22" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
         <v>10</v>
       </c>
@@ -1170,20 +1247,23 @@
       <c r="D23" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23">
+        <v>20</v>
+      </c>
+      <c r="F23" s="3">
         <v>44945</v>
       </c>
-      <c r="F23" s="4">
+      <c r="G23" s="4">
         <v>0.93055555555555558</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H23" s="1">
         <v>22</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I23" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
         <v>11</v>
       </c>
@@ -1196,20 +1276,23 @@
       <c r="D24" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24">
+        <v>20</v>
+      </c>
+      <c r="F24" s="3">
         <v>44949</v>
       </c>
-      <c r="F24" s="4">
+      <c r="G24" s="4">
         <v>0.57291666666666663</v>
       </c>
-      <c r="G24" s="1">
+      <c r="H24" s="1">
         <v>37</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I24" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2">
         <v>12</v>
       </c>
@@ -1222,20 +1305,23 @@
       <c r="D25" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25">
+        <v>21</v>
+      </c>
+      <c r="F25" s="3">
         <v>44952</v>
       </c>
-      <c r="F25" s="4">
+      <c r="G25" s="4">
         <v>0.375</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
         <v>29</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I25" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
         <v>13</v>
       </c>
@@ -1248,20 +1334,23 @@
       <c r="D26" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26">
+        <v>20</v>
+      </c>
+      <c r="F26" s="3">
         <v>44952</v>
       </c>
-      <c r="F26" s="5">
+      <c r="G26" s="5">
         <v>0.41666666666666669</v>
       </c>
-      <c r="G26" s="1">
+      <c r="H26" s="1">
         <v>30</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I26" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
         <v>14</v>
       </c>
@@ -1274,23 +1363,26 @@
       <c r="D27" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27">
+        <v>22</v>
+      </c>
+      <c r="F27" s="3">
         <v>44952</v>
       </c>
-      <c r="F27" s="4">
+      <c r="G27" s="4">
         <v>0.45833333333333331</v>
       </c>
-      <c r="G27" s="1">
+      <c r="H27" s="1">
         <v>31</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="I27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J27" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
         <v>15</v>
       </c>
@@ -1303,20 +1395,23 @@
       <c r="D28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28">
+        <v>20</v>
+      </c>
+      <c r="F28" s="3">
         <v>44953</v>
       </c>
-      <c r="F28" s="4">
+      <c r="G28" s="4">
         <v>0.375</v>
       </c>
-      <c r="G28" s="1">
+      <c r="H28" s="1">
         <v>36</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I28" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
         <v>16</v>
       </c>
@@ -1329,20 +1424,23 @@
       <c r="D29" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29">
+        <v>20</v>
+      </c>
+      <c r="F29" s="3">
         <v>44953</v>
       </c>
-      <c r="F29" s="4">
+      <c r="G29" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="G29" s="1">
+      <c r="H29" s="1">
         <v>19</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I29" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
         <v>17</v>
       </c>
@@ -1355,23 +1453,26 @@
       <c r="D30" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30">
+        <v>21</v>
+      </c>
+      <c r="F30" s="3">
         <v>44953</v>
       </c>
-      <c r="F30" s="4">
+      <c r="G30" s="4">
         <v>0.45833333333333331</v>
       </c>
-      <c r="G30" s="1">
+      <c r="H30" s="1">
         <v>25</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="I30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J30" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
         <v>18</v>
       </c>
@@ -1384,20 +1485,23 @@
       <c r="D31" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31">
+        <v>19</v>
+      </c>
+      <c r="F31" s="3">
         <v>44956</v>
       </c>
-      <c r="F31" s="4">
+      <c r="G31" s="4">
         <v>0.375</v>
       </c>
-      <c r="G31" s="1">
+      <c r="H31" s="1">
         <v>35</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I31" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
         <v>19</v>
       </c>
@@ -1410,20 +1514,23 @@
       <c r="D32" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32">
+        <v>29</v>
+      </c>
+      <c r="F32" s="3">
         <v>44956</v>
       </c>
-      <c r="F32" s="4">
+      <c r="G32" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="G32" s="1">
+      <c r="H32" s="1">
         <v>22</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I32" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
         <v>20</v>
       </c>
@@ -1436,23 +1543,26 @@
       <c r="D33" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33">
+        <v>22</v>
+      </c>
+      <c r="F33" s="3">
         <v>44957</v>
       </c>
-      <c r="F33" s="4">
+      <c r="G33" s="4">
         <v>0.52083333333333337</v>
       </c>
-      <c r="G33" s="1">
+      <c r="H33" s="1">
         <v>30</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="I33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J33" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2">
         <v>21</v>
       </c>
@@ -1465,20 +1575,23 @@
       <c r="D34" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34">
+        <v>19</v>
+      </c>
+      <c r="F34" s="3">
         <v>44956</v>
       </c>
-      <c r="F34" s="4">
+      <c r="G34" s="4">
         <v>0.5625</v>
       </c>
-      <c r="G34" s="1">
+      <c r="H34" s="1">
         <v>31</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I34" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2">
         <v>22</v>
       </c>
@@ -1491,20 +1604,23 @@
       <c r="D35" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35">
+        <v>20</v>
+      </c>
+      <c r="F35" s="3">
         <v>44956</v>
       </c>
-      <c r="F35" s="4">
+      <c r="G35" s="4">
         <v>0.60416666666666663</v>
       </c>
-      <c r="G35" s="1">
+      <c r="H35" s="1">
         <v>23</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I35" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2">
         <v>23</v>
       </c>
@@ -1517,20 +1633,23 @@
       <c r="D36" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36">
+        <v>22</v>
+      </c>
+      <c r="F36" s="3">
         <v>44958</v>
       </c>
-      <c r="F36" s="4">
+      <c r="G36" s="4">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G36" s="1">
+      <c r="H36" s="1">
         <v>31</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I36" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2">
         <v>24</v>
       </c>
@@ -1543,20 +1662,23 @@
       <c r="D37" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37">
+        <v>21</v>
+      </c>
+      <c r="F37" s="3">
         <v>44958</v>
       </c>
-      <c r="F37" s="4">
+      <c r="G37" s="4">
         <v>0.625</v>
       </c>
-      <c r="G37" s="1">
+      <c r="H37" s="1">
         <v>18</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I37" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="2">
         <v>25</v>
       </c>
@@ -1569,20 +1691,23 @@
       <c r="D38" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38">
+        <v>21</v>
+      </c>
+      <c r="F38" s="3">
         <v>44959</v>
       </c>
-      <c r="F38" s="4">
+      <c r="G38" s="4">
         <v>0.4375</v>
       </c>
-      <c r="G38" s="1">
+      <c r="H38" s="1">
         <v>18</v>
       </c>
-      <c r="H38" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I38" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="2">
         <v>26</v>
       </c>
@@ -1595,20 +1720,20 @@
       <c r="D39" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E39" s="3">
+      <c r="F39" s="3">
         <v>44960</v>
       </c>
-      <c r="F39" s="4">
+      <c r="G39" s="4">
         <v>0.5</v>
       </c>
-      <c r="G39" s="1">
+      <c r="H39" s="1">
         <v>47</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I39" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="2">
         <v>27</v>
       </c>
@@ -1621,20 +1746,23 @@
       <c r="D40" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40">
+        <v>20</v>
+      </c>
+      <c r="F40" s="3">
         <v>44963</v>
       </c>
-      <c r="F40" s="4">
+      <c r="G40" s="4">
         <v>0.38541666666666669</v>
       </c>
-      <c r="G40" s="1">
+      <c r="H40" s="1">
         <v>21</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I40" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="2">
         <v>28</v>
       </c>
@@ -1647,20 +1775,23 @@
       <c r="D41" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41">
+        <v>18</v>
+      </c>
+      <c r="F41" s="3">
         <v>44963</v>
       </c>
-      <c r="F41" s="4">
+      <c r="G41" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="G41" s="1">
+      <c r="H41" s="1">
         <v>28</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I41" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
         <v>29</v>
       </c>
@@ -1673,20 +1804,23 @@
       <c r="D42" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42">
+        <v>21</v>
+      </c>
+      <c r="F42" s="3">
         <v>44963</v>
       </c>
-      <c r="F42" s="4">
+      <c r="G42" s="4">
         <v>0.58333333333333337</v>
       </c>
-      <c r="G42" s="1">
+      <c r="H42" s="1">
         <v>29</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I42" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="2">
         <v>30</v>
       </c>
@@ -1699,20 +1833,23 @@
       <c r="D43" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43">
+        <v>19</v>
+      </c>
+      <c r="F43" s="3">
         <v>44964</v>
       </c>
-      <c r="F43" s="4">
+      <c r="G43" s="4">
         <v>0.39583333333333331</v>
       </c>
-      <c r="G43" s="1">
+      <c r="H43" s="1">
         <v>24</v>
       </c>
-      <c r="H43" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I43" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="2">
         <v>31</v>
       </c>
@@ -1725,20 +1862,23 @@
       <c r="D44" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44">
+        <v>23</v>
+      </c>
+      <c r="F44" s="3">
         <v>44964</v>
       </c>
-      <c r="F44" s="4">
+      <c r="G44" s="4">
         <v>0.5625</v>
       </c>
-      <c r="G44" s="1">
+      <c r="H44" s="1">
         <v>43</v>
       </c>
-      <c r="H44" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I44" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1">
         <v>32</v>
       </c>
@@ -1751,20 +1891,33 @@
       <c r="D45" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45">
+        <v>20</v>
+      </c>
+      <c r="F45" s="3">
         <v>44967</v>
       </c>
-      <c r="F45" s="4">
+      <c r="G45" s="4">
         <v>0.4375</v>
       </c>
-      <c r="G45" s="1">
-        <v>20</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>49</v>
+      <c r="H45" s="1">
+        <v>20</v>
       </c>
       <c r="I45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J45" s="1" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E47">
+        <f>AVERAGE(E4:E6,E16:E19,E21:E44)</f>
+        <v>21.206896551724139</v>
+      </c>
+      <c r="F47">
+        <f>STDEV(E4:E6,E16:E19,E21:E45)</f>
+        <v>2.492517538185218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>